<commit_message>
Updated path to test data and path of test data file in base.
</commit_message>
<xml_diff>
--- a/com.automationpractice/src/main/java/com/automationpractice/testdata/AutomationPracticeTestData.xlsx
+++ b/com.automationpractice/src/main/java/com/automationpractice/testdata/AutomationPracticeTestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\eclipse-workspace\com.automationpractice\src\main\java\com\automationpractice\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\git\AutomationPractice\com.automationpractice\src\main\java\com\automationpractice\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E343C54C-2586-4779-A708-2C91E1065437}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{98D830B7-9ADA-4FE0-9C5E-3C11D345BDFF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{BC3AF89F-1EFC-4B37-A16D-C58A2F1DB57D}"/>
   </bookViews>
@@ -123,28 +123,28 @@
     <t>Mrs.</t>
   </si>
   <si>
-    <t>FN1@LN1.com</t>
-  </si>
-  <si>
-    <t>FN2@LN2.com</t>
-  </si>
-  <si>
     <t>FN3@LN3.com</t>
   </si>
   <si>
-    <t>FN4@LN4.com</t>
-  </si>
-  <si>
     <t>FN5@LN5.com</t>
   </si>
   <si>
-    <t>FN6@LN6.com</t>
-  </si>
-  <si>
     <t>FN</t>
   </si>
   <si>
     <t>LN</t>
+  </si>
+  <si>
+    <t>FN7@LN7.com</t>
+  </si>
+  <si>
+    <t>FN8@LN8.com</t>
+  </si>
+  <si>
+    <t>FN9@LN9.com</t>
+  </si>
+  <si>
+    <t>FN12@LN12.com</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -588,13 +588,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>
@@ -609,10 +609,10 @@
         <v>1988</v>
       </c>
       <c r="I2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -638,13 +638,13 @@
         <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>17</v>
@@ -659,10 +659,10 @@
         <v>1988</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
         <v>26</v>
@@ -688,13 +688,13 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
         <v>17</v>
@@ -709,10 +709,10 @@
         <v>1988</v>
       </c>
       <c r="I4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
@@ -738,13 +738,13 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -759,10 +759,10 @@
         <v>1988</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
         <v>28</v>
@@ -788,13 +788,13 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
@@ -809,10 +809,10 @@
         <v>1988</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
         <v>29</v>
@@ -838,13 +838,13 @@
         <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -859,10 +859,10 @@
         <v>1988</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="K7" t="s">
         <v>30</v>

</xml_diff>